<commit_message>
feat: Generalize class assignment for dynamic inputs
- Auto-detect input class count from Excel sheets

- Add GUI input for target output class count

- Update logic to support N classes

- Update tests and documentation
</commit_message>
<xml_diff>
--- a/01 5학년_가상 명단.xlsx
+++ b/01 5학년_가상 명단.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11116"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11130"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kwansooahn/WorkSpace/Class_Assignment 2/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF6A0D7E-407A-644D-A21A-357C53F3B27B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE008442-64A5-2F42-BAC9-C3ECB6CF00A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19920" yWindow="2040" windowWidth="20140" windowHeight="15920" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="18260" yWindow="2040" windowWidth="20140" windowHeight="15920" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="5-1" sheetId="3" r:id="rId1"/>
@@ -20,7 +20,6 @@
     <sheet name="5-5" sheetId="6" r:id="rId5"/>
     <sheet name="5-6" sheetId="5" r:id="rId6"/>
     <sheet name="5-7" sheetId="7" r:id="rId7"/>
-    <sheet name="Sheet2" sheetId="9" r:id="rId8"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -5112,7 +5111,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{08A5934A-3E40-40AC-8CF0-DF85939892FB}">
   <dimension ref="A1:J23"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="G26" sqref="G26"/>
     </sheetView>
   </sheetViews>
@@ -5712,76 +5711,4 @@
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <legacyDrawing r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{531FC5E2-A331-394D-8598-89A3F3E74953}">
-  <dimension ref="A1:B7"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E24" sqref="E24"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="17"/>
-  <sheetData>
-    <row r="1" spans="1:2">
-      <c r="A1">
-        <v>1</v>
-      </c>
-      <c r="B1">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2">
-      <c r="A2">
-        <v>2</v>
-      </c>
-      <c r="B2">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2">
-      <c r="A3">
-        <v>3</v>
-      </c>
-      <c r="B3">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2">
-      <c r="A4">
-        <v>4</v>
-      </c>
-      <c r="B4">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2">
-      <c r="A5">
-        <v>5</v>
-      </c>
-      <c r="B5">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2">
-      <c r="A6">
-        <v>6</v>
-      </c>
-      <c r="B6">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2">
-      <c r="A7">
-        <v>7</v>
-      </c>
-      <c r="B7">
-        <v>22</v>
-      </c>
-    </row>
-  </sheetData>
-  <phoneticPr fontId="3" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>